<commit_message>
Added grades and notes to assignment sheet
</commit_message>
<xml_diff>
--- a/assignments/assignments_sheet.xlsx
+++ b/assignments/assignments_sheet.xlsx
@@ -5,18 +5,18 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/liviosilva-muller/Documents/GitHub/Fundamentals_of_R_IHEID2022/assignments/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/henriquesposito/Documents/GitHub/Fundamentals_of_R_IHEID2022/assignments/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{C92F14FE-A01F-7E44-AA4C-C75D0BF14683}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{12943316-23BE-5543-B5E3-ECB3753F9B2C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-5480" yWindow="-21600" windowWidth="38400" windowHeight="21600" xr2:uid="{F18C4139-FD07-6E4A-A40C-D8602D7A0A6F}"/>
+    <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="17560" xr2:uid="{F18C4139-FD07-6E4A-A40C-D8602D7A0A6F}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$J$1</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$L$1</definedName>
   </definedNames>
   <calcPr calcId="181029"/>
   <extLst>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="35">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="45">
   <si>
     <t>Student</t>
   </si>
@@ -144,6 +144,36 @@
   </si>
   <si>
     <t>f_a_on_time</t>
+  </si>
+  <si>
+    <t>Grade HS</t>
+  </si>
+  <si>
+    <t>Notes HM1</t>
+  </si>
+  <si>
+    <t>Issues with turnout and subsetting</t>
+  </si>
+  <si>
+    <t>Missing the last few questions… subseting issue?</t>
+  </si>
+  <si>
+    <t>Issue with subsetting</t>
+  </si>
+  <si>
+    <t>Sent in 2 scripts, no comments… All appears to be correct but I do not understand…</t>
+  </si>
+  <si>
+    <t>Managed to do everything, but answers for lest few exercises are wrong…</t>
+  </si>
+  <si>
+    <t>Could not do last two exercises</t>
+  </si>
+  <si>
+    <t>Appears to have done everything corretly, answers are confusing though… Also sent in two files, one R script for first exercise and the other ion rmd.</t>
+  </si>
+  <si>
+    <t>Are we sure she is not in?</t>
   </si>
 </sst>
 </file>
@@ -545,26 +575,27 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3BCFC498-9AAB-094A-B31F-54AAE91DF5DE}">
-  <dimension ref="A1:J26"/>
+  <dimension ref="A1:L26"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L9" sqref="L9"/>
+      <selection activeCell="F21" sqref="F21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="39.5" style="2" customWidth="1"/>
-    <col min="3" max="3" width="16.83203125" customWidth="1"/>
-    <col min="4" max="4" width="20.1640625" customWidth="1"/>
-    <col min="5" max="5" width="17" customWidth="1"/>
-    <col min="6" max="6" width="18.83203125" customWidth="1"/>
-    <col min="7" max="7" width="15" customWidth="1"/>
-    <col min="8" max="8" width="14.83203125" customWidth="1"/>
-    <col min="9" max="9" width="19" customWidth="1"/>
-    <col min="10" max="10" width="12.83203125" customWidth="1"/>
+    <col min="3" max="4" width="16.83203125" customWidth="1"/>
+    <col min="5" max="5" width="20.1640625" customWidth="1"/>
+    <col min="6" max="6" width="37" customWidth="1"/>
+    <col min="7" max="7" width="17" customWidth="1"/>
+    <col min="8" max="8" width="18.83203125" customWidth="1"/>
+    <col min="9" max="9" width="15" customWidth="1"/>
+    <col min="10" max="10" width="14.83203125" customWidth="1"/>
+    <col min="11" max="11" width="19" customWidth="1"/>
+    <col min="12" max="12" width="12.83203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" s="4" customFormat="1" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:12" s="4" customFormat="1" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
@@ -575,28 +606,34 @@
         <v>27</v>
       </c>
       <c r="D1" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="E1" s="4" t="s">
         <v>31</v>
       </c>
-      <c r="E1" s="4" t="s">
+      <c r="F1" s="4" t="s">
+        <v>36</v>
+      </c>
+      <c r="G1" s="4" t="s">
         <v>28</v>
       </c>
-      <c r="F1" s="4" t="s">
+      <c r="H1" s="4" t="s">
         <v>32</v>
       </c>
-      <c r="G1" s="4" t="s">
+      <c r="I1" s="4" t="s">
         <v>29</v>
       </c>
-      <c r="H1" s="4" t="s">
+      <c r="J1" s="4" t="s">
         <v>33</v>
       </c>
-      <c r="I1" s="4" t="s">
+      <c r="K1" s="4" t="s">
         <v>30</v>
       </c>
-      <c r="J1" s="4" t="s">
+      <c r="L1" s="4" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="2" spans="1:10" ht="18" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:12" ht="18" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>1</v>
       </c>
@@ -604,10 +641,16 @@
         <v>0</v>
       </c>
       <c r="D2">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="3" spans="1:10" ht="18" thickBot="1" x14ac:dyDescent="0.25">
+        <v>5.5</v>
+      </c>
+      <c r="E2">
+        <v>1</v>
+      </c>
+      <c r="F2" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="3" spans="1:12" ht="18" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>2</v>
       </c>
@@ -615,10 +658,13 @@
         <v>0</v>
       </c>
       <c r="D3">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="4" spans="1:10" ht="18" thickBot="1" x14ac:dyDescent="0.25">
+        <v>6</v>
+      </c>
+      <c r="E3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:12" ht="18" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>3</v>
       </c>
@@ -626,10 +672,13 @@
         <v>0</v>
       </c>
       <c r="D4">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="5" spans="1:10" ht="18" thickBot="1" x14ac:dyDescent="0.25">
+        <v>6</v>
+      </c>
+      <c r="E4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:12" ht="18" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
         <v>4</v>
       </c>
@@ -637,10 +686,13 @@
         <v>0</v>
       </c>
       <c r="D5">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="6" spans="1:10" ht="18" thickBot="1" x14ac:dyDescent="0.25">
+        <v>6</v>
+      </c>
+      <c r="E5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:12" ht="18" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
         <v>5</v>
       </c>
@@ -648,10 +700,13 @@
         <v>0</v>
       </c>
       <c r="D6">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="7" spans="1:10" ht="18" thickBot="1" x14ac:dyDescent="0.25">
+        <v>6</v>
+      </c>
+      <c r="E6">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" spans="1:12" ht="18" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
         <v>6</v>
       </c>
@@ -659,10 +714,16 @@
         <v>0</v>
       </c>
       <c r="D7">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="8" spans="1:10" ht="18" thickBot="1" x14ac:dyDescent="0.25">
+        <v>5</v>
+      </c>
+      <c r="E7">
+        <v>1</v>
+      </c>
+      <c r="F7" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="8" spans="1:12" ht="18" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
         <v>7</v>
       </c>
@@ -670,10 +731,16 @@
         <v>0</v>
       </c>
       <c r="D8">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="9" spans="1:10" ht="18" thickBot="1" x14ac:dyDescent="0.25">
+        <v>0</v>
+      </c>
+      <c r="E8">
+        <v>0</v>
+      </c>
+      <c r="F8" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="9" spans="1:12" ht="18" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
         <v>8</v>
       </c>
@@ -681,10 +748,13 @@
         <v>0</v>
       </c>
       <c r="D9">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="10" spans="1:10" ht="18" thickBot="1" x14ac:dyDescent="0.25">
+        <v>5.5</v>
+      </c>
+      <c r="E9">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="10" spans="1:12" ht="18" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
         <v>9</v>
       </c>
@@ -692,10 +762,16 @@
         <v>0</v>
       </c>
       <c r="D10">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="11" spans="1:10" ht="18" thickBot="1" x14ac:dyDescent="0.25">
+        <v>5.5</v>
+      </c>
+      <c r="E10">
+        <v>1</v>
+      </c>
+      <c r="F10" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="11" spans="1:12" ht="18" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
         <v>10</v>
       </c>
@@ -703,21 +779,28 @@
         <v>0</v>
       </c>
       <c r="D11">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="12" spans="1:10" ht="18" thickBot="1" x14ac:dyDescent="0.25">
+        <v>6</v>
+      </c>
+      <c r="E11">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="12" spans="1:12" ht="18" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
         <v>11</v>
       </c>
       <c r="B12">
         <v>0</v>
       </c>
-      <c r="D12" s="5">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="13" spans="1:10" ht="18" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="D12">
+        <v>0</v>
+      </c>
+      <c r="E12" s="5">
+        <v>0</v>
+      </c>
+      <c r="F12" s="5"/>
+    </row>
+    <row r="13" spans="1:12" ht="18" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
         <v>12</v>
       </c>
@@ -725,10 +808,13 @@
         <v>0</v>
       </c>
       <c r="D13">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="14" spans="1:10" ht="18" thickBot="1" x14ac:dyDescent="0.25">
+        <v>6</v>
+      </c>
+      <c r="E13">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="14" spans="1:12" ht="18" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
         <v>13</v>
       </c>
@@ -736,10 +822,13 @@
         <v>0</v>
       </c>
       <c r="D14">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="15" spans="1:10" ht="18" thickBot="1" x14ac:dyDescent="0.25">
+        <v>6</v>
+      </c>
+      <c r="E14">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="15" spans="1:12" ht="18" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
         <v>14</v>
       </c>
@@ -747,10 +836,16 @@
         <v>0</v>
       </c>
       <c r="D15">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="16" spans="1:10" ht="18" thickBot="1" x14ac:dyDescent="0.25">
+        <v>5.5</v>
+      </c>
+      <c r="E15">
+        <v>1</v>
+      </c>
+      <c r="F15" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="16" spans="1:12" ht="18" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A16" s="1" t="s">
         <v>15</v>
       </c>
@@ -758,10 +853,13 @@
         <v>0</v>
       </c>
       <c r="D16">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="17" spans="1:4" ht="18" thickBot="1" x14ac:dyDescent="0.25">
+        <v>6</v>
+      </c>
+      <c r="E16">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" ht="18" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A17" s="1" t="s">
         <v>16</v>
       </c>
@@ -769,10 +867,16 @@
         <v>0</v>
       </c>
       <c r="D17">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="18" spans="1:4" ht="18" thickBot="1" x14ac:dyDescent="0.25">
+        <v>5.5</v>
+      </c>
+      <c r="E17">
+        <v>1</v>
+      </c>
+      <c r="F17" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" ht="18" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A18" s="1" t="s">
         <v>17</v>
       </c>
@@ -780,21 +884,31 @@
         <v>0</v>
       </c>
       <c r="D18">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="19" spans="1:4" ht="18" thickBot="1" x14ac:dyDescent="0.25">
+        <v>6</v>
+      </c>
+      <c r="E18">
+        <v>1</v>
+      </c>
+      <c r="F18" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" ht="18" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A19" s="1" t="s">
         <v>18</v>
       </c>
       <c r="B19">
         <v>0</v>
       </c>
-      <c r="D19" s="5">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="20" spans="1:4" ht="18" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="D19">
+        <v>0</v>
+      </c>
+      <c r="E19" s="5">
+        <v>0</v>
+      </c>
+      <c r="F19" s="5"/>
+    </row>
+    <row r="20" spans="1:6" ht="18" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A20" s="1" t="s">
         <v>19</v>
       </c>
@@ -802,10 +916,16 @@
         <v>1</v>
       </c>
       <c r="D20">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="21" spans="1:4" ht="18" thickBot="1" x14ac:dyDescent="0.25">
+        <v>6</v>
+      </c>
+      <c r="E20">
+        <v>1</v>
+      </c>
+      <c r="F20" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6" ht="18" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A21" s="1" t="s">
         <v>20</v>
       </c>
@@ -815,8 +935,11 @@
       <c r="D21">
         <v>0</v>
       </c>
-    </row>
-    <row r="22" spans="1:4" ht="18" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="E21">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6" ht="18" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A22" s="1" t="s">
         <v>21</v>
       </c>
@@ -826,8 +949,11 @@
       <c r="D22">
         <v>0</v>
       </c>
-    </row>
-    <row r="23" spans="1:4" ht="18" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="E22">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6" ht="18" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A23" s="1" t="s">
         <v>22</v>
       </c>
@@ -837,8 +963,11 @@
       <c r="D23">
         <v>0</v>
       </c>
-    </row>
-    <row r="24" spans="1:4" ht="18" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="E23">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6" ht="18" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A24" s="1" t="s">
         <v>23</v>
       </c>
@@ -848,8 +977,11 @@
       <c r="D24">
         <v>0</v>
       </c>
-    </row>
-    <row r="25" spans="1:4" ht="18" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="E24">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6" ht="18" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A25" s="1" t="s">
         <v>24</v>
       </c>
@@ -859,8 +991,11 @@
       <c r="D25">
         <v>0</v>
       </c>
-    </row>
-    <row r="26" spans="1:4" ht="18" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="E25">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="26" spans="1:6" ht="18" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A26" s="1" t="s">
         <v>25</v>
       </c>
@@ -870,9 +1005,12 @@
       <c r="D26">
         <v>0</v>
       </c>
+      <c r="E26">
+        <v>0</v>
+      </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:J1" xr:uid="{3BCFC498-9AAB-094A-B31F-54AAE91DF5DE}"/>
+  <autoFilter ref="A1:L1" xr:uid="{3BCFC498-9AAB-094A-B31F-54AAE91DF5DE}"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Updated grading in assignments sheet
</commit_message>
<xml_diff>
--- a/assignments/assignments_sheet.xlsx
+++ b/assignments/assignments_sheet.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/henriquesposito/Documents/GitHub/Fundamentals_of_R_IHEID2022/assignments/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{80FD6338-F32B-C241-A3E5-3C18E067A39F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{31F8903E-A41A-F64C-A2B5-85C33BA8AC51}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="17560" xr2:uid="{F18C4139-FD07-6E4A-A40C-D8602D7A0A6F}"/>
   </bookViews>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="48">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="46">
   <si>
     <t>Student</t>
   </si>
@@ -173,13 +173,7 @@
     <t>Appears to have done everything corretly, answers are confusing though… Also sent in two files, one R script for first exercise and the other ion rmd.</t>
   </si>
   <si>
-    <t>Are we sure she is not in?</t>
-  </si>
-  <si>
     <t>Had a bike accident, turned in late but all is correct. She was also in office hours. Get full grade.</t>
-  </si>
-  <si>
-    <t>Are we sure she is not auditing?</t>
   </si>
   <si>
     <t>Submitted late without a proper excuse… also, several things appear missing…</t>
@@ -569,10 +563,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3BCFC498-9AAB-094A-B31F-54AAE91DF5DE}">
-  <dimension ref="A1:L26"/>
+  <dimension ref="A1:L27"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F9" sqref="F9"/>
+      <selection activeCell="E12" sqref="E12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -635,7 +629,7 @@
         <v>0</v>
       </c>
       <c r="D2">
-        <v>5.5</v>
+        <v>5.75</v>
       </c>
       <c r="E2">
         <v>1</v>
@@ -708,7 +702,7 @@
         <v>0</v>
       </c>
       <c r="D7">
-        <v>5</v>
+        <v>5.75</v>
       </c>
       <c r="E7">
         <v>1</v>
@@ -725,13 +719,13 @@
         <v>0</v>
       </c>
       <c r="D8">
-        <v>4.75</v>
+        <v>5</v>
       </c>
       <c r="E8">
         <v>0</v>
       </c>
       <c r="F8" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
     </row>
     <row r="9" spans="1:12" ht="18" thickBot="1" x14ac:dyDescent="0.25">
@@ -742,7 +736,7 @@
         <v>0</v>
       </c>
       <c r="D9">
-        <v>5.5</v>
+        <v>5.75</v>
       </c>
       <c r="E9">
         <v>1</v>
@@ -759,7 +753,7 @@
         <v>0</v>
       </c>
       <c r="D10">
-        <v>5.5</v>
+        <v>5.75</v>
       </c>
       <c r="E10">
         <v>1</v>
@@ -796,7 +790,7 @@
         <v>0</v>
       </c>
       <c r="F12" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
     </row>
     <row r="13" spans="1:12" ht="18" thickBot="1" x14ac:dyDescent="0.25">
@@ -835,7 +829,7 @@
         <v>0</v>
       </c>
       <c r="D15">
-        <v>5.5</v>
+        <v>5.75</v>
       </c>
       <c r="E15">
         <v>1</v>
@@ -866,7 +860,7 @@
         <v>0</v>
       </c>
       <c r="D17">
-        <v>5.5</v>
+        <v>5.75</v>
       </c>
       <c r="E17">
         <v>1</v>
@@ -894,41 +888,24 @@
     </row>
     <row r="19" spans="1:6" ht="18" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A19" s="1" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="B19">
         <v>0</v>
       </c>
       <c r="D19">
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="E19">
-        <v>0</v>
-      </c>
-      <c r="F19" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="20" spans="1:6" ht="18" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A20" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="B20">
-        <v>1</v>
-      </c>
-      <c r="D20">
-        <v>6</v>
-      </c>
-      <c r="E20">
-        <v>1</v>
-      </c>
-      <c r="F20" t="s">
-        <v>44</v>
-      </c>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A20" s="1"/>
     </row>
     <row r="21" spans="1:6" ht="18" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A21" s="1" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="B21">
         <v>1</v>
@@ -942,7 +919,7 @@
     </row>
     <row r="22" spans="1:6" ht="18" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A22" s="1" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B22">
         <v>1</v>
@@ -956,7 +933,7 @@
     </row>
     <row r="23" spans="1:6" ht="18" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A23" s="1" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B23">
         <v>1</v>
@@ -970,7 +947,7 @@
     </row>
     <row r="24" spans="1:6" ht="18" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A24" s="1" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B24">
         <v>1</v>
@@ -984,7 +961,7 @@
     </row>
     <row r="25" spans="1:6" ht="18" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A25" s="1" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B25">
         <v>1</v>
@@ -998,15 +975,29 @@
     </row>
     <row r="26" spans="1:6" ht="18" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A26" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="B26">
+        <v>1</v>
+      </c>
+      <c r="D26">
+        <v>0</v>
+      </c>
+      <c r="E26">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="27" spans="1:6" ht="18" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A27" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="B26">
-        <v>1</v>
-      </c>
-      <c r="D26">
-        <v>0</v>
-      </c>
-      <c r="E26">
+      <c r="B27">
+        <v>1</v>
+      </c>
+      <c r="D27">
+        <v>0</v>
+      </c>
+      <c r="E27">
         <v>0</v>
       </c>
     </row>

</xml_diff>